<commit_message>
#Adicionar e Cadastrar Com Sucesso
</commit_message>
<xml_diff>
--- a/Arquivos/Compras.xlsx
+++ b/Arquivos/Compras.xlsx
@@ -7,37 +7,69 @@
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
-    <sheet name="Estoque" sheetId="1" r:id="rId1"/>
+    <sheet name="Produtos" sheetId="1" r:id="rId1"/>
+    <sheet name="Estoque" sheetId="2" r:id="rId2"/>
+    <sheet name="Vendas" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
-  <si>
-    <t>Tipo de Produto</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="18">
+  <si>
+    <t>Produto</t>
   </si>
   <si>
     <t>Marca</t>
   </si>
   <si>
+    <t>Método_Compra</t>
+  </si>
+  <si>
+    <t>Valor_Método</t>
+  </si>
+  <si>
+    <t>Método_Venda</t>
+  </si>
+  <si>
+    <t>Ração</t>
+  </si>
+  <si>
+    <t>Shampoo</t>
+  </si>
+  <si>
+    <t>Pedigree</t>
+  </si>
+  <si>
+    <t>Gato</t>
+  </si>
+  <si>
+    <t>Pacote</t>
+  </si>
+  <si>
+    <t>Unidade</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
     <t>Quantidade</t>
   </si>
   <si>
     <t>Valor Total Gasto</t>
   </si>
   <si>
-    <t>Ração</t>
-  </si>
-  <si>
-    <t>Pedigree</t>
-  </si>
-  <si>
-    <t>2</t>
+    <t>6</t>
+  </si>
+  <si>
+    <t>100</t>
   </si>
   <si>
     <t>20.0</t>
+  </si>
+  <si>
+    <t>2.0</t>
   </si>
 </sst>
 </file>
@@ -395,9 +427,70 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:D4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
@@ -409,24 +502,69 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>3</v>
+        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" t="s">
         <v>5</v>
       </c>
-      <c r="C2" t="s">
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" t="s">
         <v>6</v>
       </c>
-      <c r="D2" t="s">
-        <v>7</v>
+      <c r="B4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" t="s">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
#Começo da janela Vender
</commit_message>
<xml_diff>
--- a/Arquivos/Compras.xlsx
+++ b/Arquivos/Compras.xlsx
@@ -10,13 +10,14 @@
     <sheet name="Produtos" sheetId="1" r:id="rId1"/>
     <sheet name="Estoque" sheetId="2" r:id="rId2"/>
     <sheet name="Vendas" sheetId="3" r:id="rId3"/>
+    <sheet name="Métodos" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="14">
   <si>
     <t>Produto</t>
   </si>
@@ -36,22 +37,13 @@
     <t>Ração</t>
   </si>
   <si>
-    <t>Shampoo</t>
-  </si>
-  <si>
     <t>Pedigree</t>
   </si>
   <si>
-    <t>Gato</t>
-  </si>
-  <si>
     <t>Pacote</t>
   </si>
   <si>
-    <t>Unidade</t>
-  </si>
-  <si>
-    <t>2</t>
+    <t>170</t>
   </si>
   <si>
     <t>Quantidade</t>
@@ -60,16 +52,13 @@
     <t>Valor Total Gasto</t>
   </si>
   <si>
-    <t>6</t>
-  </si>
-  <si>
-    <t>100</t>
-  </si>
-  <si>
-    <t>20.0</t>
-  </si>
-  <si>
-    <t>2.0</t>
+    <t>3</t>
+  </si>
+  <si>
+    <t>510.0</t>
+  </si>
+  <si>
+    <t>Métodos</t>
   </si>
 </sst>
 </file>
@@ -427,7 +416,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -455,30 +444,16 @@
         <v>5</v>
       </c>
       <c r="B2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" t="s">
         <v>7</v>
       </c>
-      <c r="C2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D2">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5">
-      <c r="A3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" t="s">
+      <c r="D2" t="s">
         <v>8</v>
       </c>
-      <c r="C3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D3" t="s">
-        <v>11</v>
-      </c>
-      <c r="E3" t="s">
-        <v>10</v>
+      <c r="E2" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>
@@ -488,7 +463,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -502,43 +477,24 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="3" spans="1:4">
-      <c r="A3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
-      <c r="A4" t="s">
+      <c r="B2" t="s">
         <v>6</v>
       </c>
-      <c r="B4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" t="s">
-        <v>15</v>
-      </c>
-      <c r="D4" t="s">
-        <v>17</v>
+      <c r="C2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -547,6 +503,27 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:B1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B2"/>
   <sheetViews>
@@ -555,16 +532,16 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:2">
-      <c r="A1" s="1" t="s">
+      <c r="B1" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" s="1">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2">
-      <c r="A2" t="s">
-        <v>5</v>
+      <c r="B2" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
#Ultimo Commit do Dia
</commit_message>
<xml_diff>
--- a/Arquivos/Compras.xlsx
+++ b/Arquivos/Compras.xlsx
@@ -8,16 +8,13 @@
   </bookViews>
   <sheets>
     <sheet name="Produtos" sheetId="1" r:id="rId1"/>
-    <sheet name="Estoque" sheetId="2" r:id="rId2"/>
-    <sheet name="Vendas" sheetId="3" r:id="rId3"/>
-    <sheet name="Métodos" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="8">
   <si>
     <t>Produto</t>
   </si>
@@ -37,55 +34,10 @@
     <t>Ração</t>
   </si>
   <si>
-    <t>Pente</t>
-  </si>
-  <si>
     <t>Pedigree</t>
   </si>
   <si>
-    <t>Pulga</t>
-  </si>
-  <si>
     <t>Pacote</t>
-  </si>
-  <si>
-    <t>Quantidade</t>
-  </si>
-  <si>
-    <t>Valor_Unitário</t>
-  </si>
-  <si>
-    <t>Valor_Total</t>
-  </si>
-  <si>
-    <t>Valor Unitário</t>
-  </si>
-  <si>
-    <t>NumVenda</t>
-  </si>
-  <si>
-    <t>['Pente']</t>
-  </si>
-  <si>
-    <t>['Pulga']</t>
-  </si>
-  <si>
-    <t>['5']</t>
-  </si>
-  <si>
-    <t>['nan']</t>
-  </si>
-  <si>
-    <t>['Pacote']</t>
-  </si>
-  <si>
-    <t>['0']</t>
-  </si>
-  <si>
-    <t>Unnamed: 0</t>
-  </si>
-  <si>
-    <t>Métodos</t>
   </si>
 </sst>
 </file>
@@ -443,7 +395,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -471,199 +423,16 @@
         <v>5</v>
       </c>
       <c r="B2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" t="s">
         <v>7</v>
       </c>
-      <c r="C2" t="s">
-        <v>9</v>
-      </c>
       <c r="D2">
-        <v>100</v>
+        <v>10</v>
       </c>
       <c r="E2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5">
-      <c r="A3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D3">
-        <v>14</v>
-      </c>
-      <c r="E3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1" spans="1:6">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6">
-      <c r="A2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2" t="s">
         <v>7</v>
-      </c>
-      <c r="C2">
-        <v>25</v>
-      </c>
-      <c r="F2">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6">
-      <c r="A3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3">
-        <v>15</v>
-      </c>
-      <c r="F3">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6">
-      <c r="A4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4">
-        <v>14</v>
-      </c>
-      <c r="F4">
-        <v>14</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1" spans="1:7">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7">
-      <c r="A2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B2" t="s">
-        <v>16</v>
-      </c>
-      <c r="C2" t="s">
-        <v>17</v>
-      </c>
-      <c r="D2" t="s">
-        <v>18</v>
-      </c>
-      <c r="E2" t="s">
-        <v>18</v>
-      </c>
-      <c r="F2" t="s">
-        <v>19</v>
-      </c>
-      <c r="G2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1" spans="1:3">
-      <c r="A1" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3">
-      <c r="A2">
-        <v>0</v>
-      </c>
-      <c r="C2" t="s">
-        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
#Transformando em outras classes
</commit_message>
<xml_diff>
--- a/Arquivos/Compras.xlsx
+++ b/Arquivos/Compras.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="25">
   <si>
     <t>Produto</t>
   </si>
@@ -64,10 +64,7 @@
     <t>['Pacote 3kg']</t>
   </si>
   <si>
-    <t>40</t>
-  </si>
-  <si>
-    <t>20</t>
+    <t>nan</t>
   </si>
   <si>
     <t>Não</t>
@@ -500,6 +497,9 @@
       <c r="E2" t="s">
         <v>12</v>
       </c>
+      <c r="G2" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="3" spans="1:8">
       <c r="A3" t="s">
@@ -534,14 +534,14 @@
       <c r="E4" t="s">
         <v>13</v>
       </c>
-      <c r="F4" t="s">
-        <v>15</v>
-      </c>
-      <c r="G4" t="s">
+      <c r="F4">
+        <v>40</v>
+      </c>
+      <c r="G4">
+        <v>20</v>
+      </c>
+      <c r="H4" t="s">
         <v>16</v>
-      </c>
-      <c r="H4" t="s">
-        <v>17</v>
       </c>
     </row>
   </sheetData>
@@ -565,10 +565,10 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>18</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>19</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>6</v>
@@ -586,6 +586,9 @@
       </c>
       <c r="C2" t="s">
         <v>12</v>
+      </c>
+      <c r="D2" t="s">
+        <v>15</v>
       </c>
       <c r="E2">
         <v>10</v>
@@ -615,19 +618,19 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>20</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>21</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
   </sheetData>
@@ -645,7 +648,7 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:1">
@@ -655,12 +658,12 @@
     </row>
     <row r="3" spans="1:1">
       <c r="A3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
#Mais um Dia de trampo
</commit_message>
<xml_diff>
--- a/Arquivos/Compras.xlsx
+++ b/Arquivos/Compras.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="21">
   <si>
     <t>Produto</t>
   </si>
@@ -25,49 +25,31 @@
     <t>Marca</t>
   </si>
   <si>
+    <t>Valor_Venda</t>
+  </si>
+  <si>
+    <t>Valor_Compra</t>
+  </si>
+  <si>
     <t>Método_Venda</t>
   </si>
   <si>
-    <t>Valor_Método</t>
-  </si>
-  <si>
     <t>Método_Compra</t>
   </si>
   <si>
-    <t>Valor_Venda</t>
-  </si>
-  <si>
-    <t>Valor_Compra</t>
-  </si>
-  <si>
     <t>ReporEstoquepProd</t>
   </si>
   <si>
     <t>Ração</t>
   </si>
   <si>
-    <t>Shampoo</t>
-  </si>
-  <si>
     <t>Pedigree</t>
   </si>
   <si>
-    <t>Gato</t>
-  </si>
-  <si>
     <t>Pacote</t>
   </si>
   <si>
-    <t>['Pacote']</t>
-  </si>
-  <si>
-    <t>['Pacote 3kg']</t>
-  </si>
-  <si>
-    <t>nan</t>
-  </si>
-  <si>
-    <t>Não</t>
+    <t>Sim</t>
   </si>
   <si>
     <t>Método</t>
@@ -76,22 +58,28 @@
     <t>Quantidade</t>
   </si>
   <si>
-    <t>Valor_Unitário</t>
-  </si>
-  <si>
-    <t>Valor_Total</t>
-  </si>
-  <si>
-    <t>NumVenda</t>
+    <t>Num_Venda</t>
+  </si>
+  <si>
+    <t>Valor_Ganho</t>
+  </si>
+  <si>
+    <t>Frete</t>
+  </si>
+  <si>
+    <t>Desconto</t>
+  </si>
+  <si>
+    <t>Método_Pagamento</t>
+  </si>
+  <si>
+    <t>Comentário</t>
   </si>
   <si>
     <t>Métodos</t>
   </si>
   <si>
     <t>Gramas</t>
-  </si>
-  <si>
-    <t>Pacote 3kg</t>
   </si>
 </sst>
 </file>
@@ -449,13 +437,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H4"/>
+  <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:7">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -477,71 +465,28 @@
       <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" spans="1:8">
-      <c r="A2" t="s">
+      <c r="B2" t="s">
         <v>8</v>
       </c>
-      <c r="B2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C2" t="s">
-        <v>12</v>
+      <c r="C2">
+        <v>20</v>
       </c>
       <c r="D2">
         <v>10</v>
       </c>
       <c r="E2" t="s">
-        <v>12</v>
+        <v>9</v>
+      </c>
+      <c r="F2" t="s">
+        <v>9</v>
       </c>
       <c r="G2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8">
-      <c r="A3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C3" t="s">
-        <v>13</v>
-      </c>
-      <c r="E3" t="s">
-        <v>13</v>
-      </c>
-      <c r="F3">
-        <v>20</v>
-      </c>
-      <c r="G3">
         <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8">
-      <c r="A4" t="s">
-        <v>8</v>
-      </c>
-      <c r="B4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C4" t="s">
-        <v>14</v>
-      </c>
-      <c r="E4" t="s">
-        <v>13</v>
-      </c>
-      <c r="F4">
-        <v>40</v>
-      </c>
-      <c r="G4">
-        <v>20</v>
-      </c>
-      <c r="H4" t="s">
-        <v>16</v>
       </c>
     </row>
   </sheetData>
@@ -565,30 +510,30 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:6">
       <c r="A2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" t="s">
         <v>8</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2">
         <v>10</v>
-      </c>
-      <c r="C2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D2" t="s">
-        <v>15</v>
       </c>
       <c r="E2">
         <v>10</v>
@@ -604,33 +549,30 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G1"/>
+  <dimension ref="A1:F1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>18</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>21</v>
       </c>
     </row>
   </sheetData>
@@ -640,7 +582,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:A4"/>
+  <dimension ref="A1:A3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -648,22 +590,17 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" s="1" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1">
-      <c r="A4" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
# Editar Produto e Finalizar Venda pronto
</commit_message>
<xml_diff>
--- a/Arquivos/Compras.xlsx
+++ b/Arquivos/Compras.xlsx
@@ -20,12 +20,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="29">
   <si>
     <t>Método</t>
   </si>
   <si>
-    <t>Pacote</t>
+    <t>Unidade</t>
+  </si>
+  <si>
+    <t>Combo</t>
   </si>
   <si>
     <t>Produto</t>
@@ -49,10 +52,16 @@
     <t>ReporEstoquepProd</t>
   </si>
   <si>
-    <t>Ração</t>
-  </si>
-  <si>
-    <t>Pedigree</t>
+    <t>Churrasqueira</t>
+  </si>
+  <si>
+    <t>Grande</t>
+  </si>
+  <si>
+    <t>70</t>
+  </si>
+  <si>
+    <t>100</t>
   </si>
   <si>
     <t>Não</t>
@@ -88,29 +97,23 @@
     <t>Data</t>
   </si>
   <si>
-    <t>1</t>
-  </si>
-  <si>
-    <t>10</t>
-  </si>
-  <si>
-    <t>10.0</t>
-  </si>
-  <si>
-    <t>100.0</t>
-  </si>
-  <si>
-    <t>ID                    1
-Produto           Ração
-Marca          Pedigree
-Método           Pacote
-Quantidade           10
-Valor_Un           10.0
-Valor_Total       100.0
+    <t>Sim</t>
+  </si>
+  <si>
+    <t>Pix</t>
+  </si>
+  <si>
+    <t>15/01/2023</t>
+  </si>
+  <si>
+    <t>ID                         1
+Produto        Churrasqueira
+Marca               Pedigree
+Método               Unidade
+Quantidade               100
+Valor_Un                70.0
+Valor_Total           7000.0
 dtype: object</t>
-  </si>
-  <si>
-    <t>14/01/2023</t>
   </si>
 </sst>
 </file>
@@ -468,7 +471,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:A2"/>
+  <dimension ref="A1:A3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -482,6 +485,11 @@
     <row r="2" spans="1:1">
       <c r="A2" t="s">
         <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1">
+      <c r="A3" t="s">
+        <v>2</v>
       </c>
     </row>
   </sheetData>
@@ -499,48 +507,48 @@
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:7">
       <c r="A2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C2" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D2" t="s">
-        <v>1</v>
-      </c>
-      <c r="E2">
-        <v>10</v>
-      </c>
-      <c r="F2">
-        <v>30</v>
+        <v>2</v>
+      </c>
+      <c r="E2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F2" t="s">
+        <v>13</v>
       </c>
       <c r="G2" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>
@@ -550,7 +558,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G1"/>
+  <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -558,25 +566,94 @@
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" s="1" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>15</v>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2">
+        <v>10000</v>
+      </c>
+      <c r="B2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2">
+        <v>10</v>
+      </c>
+      <c r="F2">
+        <v>100</v>
+      </c>
+      <c r="G2">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3">
+        <v>10000</v>
+      </c>
+      <c r="B3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E3">
+        <v>20</v>
+      </c>
+      <c r="F3">
+        <v>100</v>
+      </c>
+      <c r="G3">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4">
+        <v>10000</v>
+      </c>
+      <c r="B4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" t="s">
+        <v>2</v>
+      </c>
+      <c r="E4">
+        <v>20</v>
+      </c>
+      <c r="F4">
+        <v>100</v>
+      </c>
+      <c r="G4">
+        <v>2000</v>
       </c>
     </row>
   </sheetData>
@@ -586,7 +663,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H1"/>
+  <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -594,28 +671,51 @@
   <sheetData>
     <row r="1" spans="1:8">
       <c r="A1" s="1" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>15</v>
-      </c>
       <c r="H1" s="1" t="s">
-        <v>21</v>
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
+      <c r="A2">
+        <v>10000</v>
+      </c>
+      <c r="B2">
+        <v>50</v>
+      </c>
+      <c r="C2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D2">
+        <v>953</v>
+      </c>
+      <c r="E2" t="s">
+        <v>26</v>
+      </c>
+      <c r="G2">
+        <v>4047</v>
+      </c>
+      <c r="H2" t="s">
+        <v>27</v>
       </c>
     </row>
   </sheetData>
@@ -633,48 +733,48 @@
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" s="1" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:7">
-      <c r="A2" t="s">
-        <v>22</v>
+      <c r="A2">
+        <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D2" t="s">
-        <v>1</v>
-      </c>
-      <c r="E2" t="s">
-        <v>23</v>
-      </c>
-      <c r="F2" t="s">
-        <v>24</v>
-      </c>
-      <c r="G2" t="s">
-        <v>25</v>
+        <v>2</v>
+      </c>
+      <c r="E2">
+        <v>100</v>
+      </c>
+      <c r="F2">
+        <v>70</v>
+      </c>
+      <c r="G2">
+        <v>7000</v>
       </c>
     </row>
   </sheetData>
@@ -692,16 +792,16 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -709,13 +809,13 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C2" t="s">
         <v>27</v>
       </c>
-      <c r="D2" t="s">
-        <v>25</v>
+      <c r="D2">
+        <v>7000</v>
       </c>
     </row>
   </sheetData>
@@ -733,30 +833,30 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C2" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D2">
-        <v>10</v>
+        <v>50</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
# Adicionar e Vender
</commit_message>
<xml_diff>
--- a/Arquivos/Compras.xlsx
+++ b/Arquivos/Compras.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="28">
   <si>
     <t>Método</t>
   </si>
@@ -28,9 +28,6 @@
     <t>Pacote</t>
   </si>
   <si>
-    <t>Unidade</t>
-  </si>
-  <si>
     <t>Produto</t>
   </si>
   <si>
@@ -55,49 +52,58 @@
     <t>Ração</t>
   </si>
   <si>
-    <t>Cachorro</t>
+    <t>Pedigree</t>
+  </si>
+  <si>
+    <t>Coelho</t>
+  </si>
+  <si>
+    <t>Não</t>
+  </si>
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>Quantidade</t>
+  </si>
+  <si>
+    <t>Valor_Un</t>
+  </si>
+  <si>
+    <t>Valor_Total</t>
+  </si>
+  <si>
+    <t>QItens</t>
+  </si>
+  <si>
+    <t>Frete</t>
+  </si>
+  <si>
+    <t>Desconto</t>
+  </si>
+  <si>
+    <t>MétodoPagamento</t>
+  </si>
+  <si>
+    <t>Comentários</t>
+  </si>
+  <si>
+    <t>Data</t>
+  </si>
+  <si>
+    <t>10001</t>
   </si>
   <si>
     <t>10</t>
   </si>
   <si>
-    <t>20</t>
-  </si>
-  <si>
-    <t>Não</t>
-  </si>
-  <si>
-    <t>ID</t>
-  </si>
-  <si>
-    <t>Quantidade</t>
-  </si>
-  <si>
-    <t>Valor_Un</t>
-  </si>
-  <si>
-    <t>Valor_Total</t>
-  </si>
-  <si>
-    <t>QItens</t>
-  </si>
-  <si>
-    <t>Frete</t>
-  </si>
-  <si>
-    <t>Desconto</t>
-  </si>
-  <si>
-    <t>MétodoPagamento</t>
-  </si>
-  <si>
-    <t>Comentários</t>
-  </si>
-  <si>
-    <t>Data</t>
-  </si>
-  <si>
-    <t>16/01/2023</t>
+    <t>70.0</t>
+  </si>
+  <si>
+    <t>700.0</t>
+  </si>
+  <si>
+    <t>17/01/2023</t>
   </si>
 </sst>
 </file>
@@ -455,7 +461,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:A3"/>
+  <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -471,11 +477,6 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:1">
-      <c r="A3" t="s">
-        <v>2</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -483,7 +484,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -491,48 +492,71 @@
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>8</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:7">
       <c r="A2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" t="s">
         <v>10</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2">
+        <v>70</v>
+      </c>
+      <c r="F2">
+        <v>80</v>
+      </c>
+      <c r="G2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" t="s">
         <v>11</v>
       </c>
-      <c r="C2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D2" t="s">
-        <v>1</v>
-      </c>
-      <c r="E2" t="s">
+      <c r="C3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E3">
+        <v>60</v>
+      </c>
+      <c r="F3">
+        <v>90</v>
+      </c>
+      <c r="G3" t="s">
         <v>12</v>
-      </c>
-      <c r="F2" t="s">
-        <v>13</v>
-      </c>
-      <c r="G2" t="s">
-        <v>14</v>
       </c>
     </row>
   </sheetData>
@@ -550,25 +574,25 @@
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>3</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>4</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>16</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>18</v>
       </c>
     </row>
   </sheetData>
@@ -586,28 +610,28 @@
   <sheetData>
     <row r="1" spans="1:8">
       <c r="A1" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="G1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>22</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>24</v>
       </c>
     </row>
   </sheetData>
@@ -617,7 +641,7 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -625,48 +649,94 @@
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>3</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>4</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>16</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:7">
       <c r="A2">
-        <v>1</v>
+        <v>10000</v>
       </c>
       <c r="B2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" t="s">
         <v>10</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2">
+        <v>20</v>
+      </c>
+      <c r="F2">
+        <v>70</v>
+      </c>
+      <c r="G2">
+        <v>1400</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3">
+        <v>10000</v>
+      </c>
+      <c r="B3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" t="s">
         <v>11</v>
       </c>
-      <c r="D2" t="s">
-        <v>1</v>
-      </c>
-      <c r="E2">
-        <v>100</v>
-      </c>
-      <c r="F2">
+      <c r="D3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E3">
         <v>10</v>
       </c>
-      <c r="G2">
-        <v>1000</v>
+      <c r="F3">
+        <v>60</v>
+      </c>
+      <c r="G3">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" t="s">
+        <v>1</v>
+      </c>
+      <c r="E4" t="s">
+        <v>24</v>
+      </c>
+      <c r="F4" t="s">
+        <v>25</v>
+      </c>
+      <c r="G4" t="s">
+        <v>26</v>
       </c>
     </row>
   </sheetData>
@@ -676,7 +746,7 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -684,30 +754,58 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2">
-        <v>1</v>
+        <v>10000</v>
       </c>
       <c r="B2">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="C2" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="D2">
-        <v>1000</v>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3">
+        <v>10000</v>
+      </c>
+      <c r="B3">
+        <v>30</v>
+      </c>
+      <c r="C3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D3">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4">
+        <v>10001</v>
+      </c>
+      <c r="B4">
+        <v>0</v>
+      </c>
+      <c r="C4" t="s">
+        <v>27</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -717,7 +815,7 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -725,30 +823,44 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>3</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>4</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" t="s">
         <v>10</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" t="s">
         <v>11</v>
       </c>
-      <c r="C2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D2">
-        <v>100</v>
+      <c r="C3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>